<commit_message>
Adding the updated lernjournal
</commit_message>
<xml_diff>
--- a/Documentation/ProjectOrganisation/team1_aufgabe3_lernjournal.xlsx
+++ b/Documentation/ProjectOrganisation/team1_aufgabe3_lernjournal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad0e591deda49bb0/Dokumente/Repos/SwissQR/swiss-qr-code/Documentation/ProjectOrganisation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marku\eclipse-workspace\swiss-qr-code\Documentation\ProjectOrganisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:40009_{44B57114-9932-4FA5-B81B-909EEB211FBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80C9BC28-4901-40E8-9170-9B9E260BD8B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82B8517-4142-48D5-9DAB-91244B8C2BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Finalisierung Aufgabe 3</t>
+  </si>
+  <si>
+    <t>Bearbeitung Aufgabe 3, Teil 1/3</t>
+  </si>
+  <si>
+    <t>Bearbeitung Aufgabe 3, Teil 2</t>
   </si>
 </sst>
 </file>
@@ -562,20 +568,20 @@
   <dimension ref="A1:IW59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="90.8984375" style="2" customWidth="1"/>
     <col min="2" max="3" width="8.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="3" customWidth="1"/>
-    <col min="5" max="17" width="10.75" style="2" customWidth="1"/>
-    <col min="18" max="257" width="10.75" style="4" customWidth="1"/>
-    <col min="258" max="1024" width="10.75" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="3" customWidth="1"/>
+    <col min="5" max="17" width="10.69921875" style="2" customWidth="1"/>
+    <col min="18" max="257" width="10.69921875" style="4" customWidth="1"/>
+    <col min="258" max="1024" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +602,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -617,7 +623,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -636,7 +642,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -655,7 +661,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -676,7 +682,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -695,7 +701,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -714,7 +720,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -737,7 +743,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -756,7 +762,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -783,9 +789,9 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" s="9">
         <v>90</v>
@@ -811,7 +817,7 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
@@ -839,14 +845,20 @@
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
     </row>
-    <row r="13" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
+    <row r="13" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <v>50</v>
+      </c>
       <c r="C13" s="10">
         <f>B13/60</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="11"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="11">
+        <v>44139</v>
+      </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -861,7 +873,7 @@
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
     </row>
-    <row r="14" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10">
@@ -883,7 +895,7 @@
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
     </row>
-    <row r="15" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -902,17 +914,17 @@
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="16">
         <f>SUM(B11:B15)</f>
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C16" s="16">
         <f>SUM(C11:C15)</f>
-        <v>2</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -929,7 +941,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -948,7 +960,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -967,7 +979,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -986,7 +998,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1021,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1028,7 +1040,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1067,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1095,7 @@
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
     </row>
-    <row r="24" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
@@ -1111,14 +1123,20 @@
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
     </row>
-    <row r="25" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
+    <row r="25" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="9">
+        <v>50</v>
+      </c>
       <c r="C25" s="10">
         <f>B25/60</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="11"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D25" s="11">
+        <v>44139</v>
+      </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -1133,7 +1151,7 @@
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
     </row>
-    <row r="26" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10">
@@ -1155,7 +1173,7 @@
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
     </row>
-    <row r="27" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1174,17 +1192,17 @@
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="16">
         <f>SUM(B23:B27)</f>
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C28" s="16">
         <f>SUM(C23:C27)</f>
-        <v>2</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1201,7 +1219,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1220,7 +1238,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1239,7 +1257,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1258,7 +1276,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>11</v>
       </c>
@@ -1281,7 +1299,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1300,7 +1318,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1345,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>12</v>
       </c>
@@ -1355,7 +1373,7 @@
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>14</v>
       </c>
@@ -1383,14 +1401,20 @@
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
     </row>
-    <row r="37" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
+    <row r="37" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="9">
+        <v>50</v>
+      </c>
       <c r="C37" s="10">
         <f>B37/60</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="11"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D37" s="11">
+        <v>44139</v>
+      </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -1405,7 +1429,7 @@
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
     </row>
-    <row r="38" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10">
@@ -1427,7 +1451,7 @@
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
     </row>
-    <row r="39" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1446,17 +1470,17 @@
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="16">
         <f>SUM(B35:B39)</f>
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C40" s="16">
         <f>SUM(C35:C39)</f>
-        <v>2</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
@@ -1473,7 +1497,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1492,7 +1516,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1511,7 +1535,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1530,7 +1554,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1549,7 +1573,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1568,7 +1592,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1587,7 +1611,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1606,7 +1630,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1625,7 +1649,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1644,7 +1668,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1663,7 +1687,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1682,7 +1706,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1701,7 +1725,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1720,7 +1744,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1739,7 +1763,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1758,7 +1782,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1777,7 +1801,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1796,7 +1820,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1815,7 +1839,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>

</xml_diff>